<commit_message>
Update BERT Custom model results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t xml:space="preserve">VECTORIZER</t>
   </si>
@@ -83,6 +83,25 @@
   </si>
   <si>
     <t xml:space="preserve">Finetuned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERT CUSTOM 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lr=2e-5
+loss=MSE
+optimizer=AdamW
+layers={bert,768,512,32,1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERT CUSTOM 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lr=2e-5
+loss=MSE
+optimizer=AdamW
+layers={bert,768,512,32,1}
+text=augmented</t>
   </si>
 </sst>
 </file>
@@ -252,14 +271,14 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.42"/>
@@ -448,7 +467,7 @@
         <v>0.3168</v>
       </c>
     </row>
-    <row r="13" s="10" customFormat="true" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="7" customFormat="true" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -475,6 +494,64 @@
       </c>
       <c r="I13" s="7" t="n">
         <v>0.4513</v>
+      </c>
+    </row>
+    <row r="15" s="7" customFormat="true" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>0.2538</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>0.1327</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>0.0295</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>0.1718</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0.515</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>0.4639</v>
+      </c>
+    </row>
+    <row r="17" s="10" customFormat="true" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>0.1818</v>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>0.1345</v>
+      </c>
+      <c r="F17" s="10" t="n">
+        <v>0.0324</v>
+      </c>
+      <c r="G17" s="10" t="n">
+        <v>0.1799</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0.5235</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>0.4698</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>